<commit_message>
updated parse_cfu and readme
</commit_message>
<xml_diff>
--- a/tests/testdata/parse_cfu/colony_counts.xlsx
+++ b/tests/testdata/parse_cfu/colony_counts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliebayne/GLabR/tests/testdata/format_cfu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliebayne/GLabR/tests/testdata/parse_cfu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B48E80-6114-E642-A9A9-AB9C28DD75CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4FB63C3-6722-8E45-93E0-4034F303B41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{4BA3F036-F8B9-7044-A189-F11F9D1D89DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Media Type</t>
   </si>
@@ -114,13 +114,76 @@
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>sample6</t>
+  </si>
+  <si>
+    <t>sample7</t>
+  </si>
+  <si>
+    <t>sample8</t>
+  </si>
+  <si>
+    <t>sample9</t>
+  </si>
+  <si>
+    <t>sample10</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>sample11</t>
+  </si>
+  <si>
+    <t>sample12</t>
+  </si>
+  <si>
+    <t>sample13</t>
+  </si>
+  <si>
+    <t>sample14</t>
+  </si>
+  <si>
+    <t>sample15</t>
+  </si>
+  <si>
+    <t>sample16</t>
+  </si>
+  <si>
+    <t>sample17</t>
+  </si>
+  <si>
+    <t>sample18</t>
+  </si>
+  <si>
+    <t>sample19</t>
+  </si>
+  <si>
+    <t>sample20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,6 +217,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="ArialMT"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -690,7 +759,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -749,37 +818,41 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q7" si="0">Q3*10</f>
         <v>100</v>
@@ -1079,34 +1152,34 @@
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1180,16 +1253,36 @@
       <c r="B21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2">
+        <v>6</v>
+      </c>
+      <c r="I21" s="2">
+        <v>7</v>
+      </c>
+      <c r="J21" s="2">
+        <v>8</v>
+      </c>
+      <c r="K21" s="2">
+        <v>9</v>
+      </c>
+      <c r="L21" s="2">
+        <v>10</v>
+      </c>
       <c r="M21" s="2"/>
       <c r="N21" s="10"/>
     </row>
@@ -1582,6 +1675,7 @@
       <c r="N41" s="14"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>